<commit_message>
SON24 new content: Charts and tables: IN12 Attainment at age 11: Review mark-ups
</commit_message>
<xml_diff>
--- a/son/content/intermediate_outcomes/compulsory_school_age_(5_to_16_years)/attainment_at_age_11/2.0/IN12-2.0-attainment-at-age-11--by-ethnicity-and-FSM--table-format.xlsx
+++ b/son/content/intermediate_outcomes/compulsory_school_age_(5_to_16_years)/attainment_at_age_11/2.0/IN12-2.0-attainment-at-age-11--by-ethnicity-and-FSM--table-format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Government Equality Hub\SON23\Code\smc-son\son\content\intermediate_outcomes\compulsory_school_age_(5_to_16_years)\attainment_at_age_11\2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9EEA63F3-E6CF-4A10-8099-7870A668D2EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5524DDE3-E364-4B94-8A81-09F6AEEAB8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="29829" windowHeight="18000" xr2:uid="{00A27BC7-2860-4489-84F7-82CD89D74D45}"/>
+    <workbookView xWindow="3771" yWindow="3771" windowWidth="24686" windowHeight="13055" xr2:uid="{00A27BC7-2860-4489-84F7-82CD89D74D45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -18,13 +18,13 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4081" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4080" uniqueCount="97">
   <si>
     <t>ind_code</t>
   </si>
@@ -311,16 +311,10 @@
     <t>West Yorkshire</t>
   </si>
   <si>
-    <t>Column Labels</t>
-  </si>
-  <si>
-    <t>Sum of value</t>
-  </si>
-  <si>
     <t>FSM eligible (%)</t>
   </si>
   <si>
-    <t>Not known to be FSM eligible (%)</t>
+    <t>Percentage (%)</t>
   </si>
 </sst>
 </file>
@@ -6367,8 +6361,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{46216E0E-190C-43A3-9B25-BBC96B04C580}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Ethnicity">
-  <location ref="A3:C21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{46216E0E-190C-43A3-9B25-BBC96B04C580}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Ethnicity">
+  <location ref="A4:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="21">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -6376,15 +6370,15 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="8">
-        <item x="1"/>
+        <item h="1" x="1"/>
         <item n="FSM eligible (%)" x="3"/>
-        <item x="5"/>
-        <item x="2"/>
-        <item n="Not known to be FSM eligible (%)" x="4"/>
-        <item x="0"/>
-        <item x="6"/>
+        <item h="1" x="5"/>
+        <item h="1" x="2"/>
+        <item n="Not known to be FSM eligible (%)" h="1" x="4"/>
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -6489,22 +6483,15 @@
       <x v="18"/>
     </i>
   </rowItems>
-  <colFields count="1">
-    <field x="6"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
+  <colItems count="1">
+    <i/>
   </colItems>
-  <pageFields count="1">
+  <pageFields count="2">
     <pageField fld="9" item="0" hier="-1"/>
+    <pageField fld="6" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Sum of value" fld="13" baseField="10" baseItem="7"/>
+    <dataField name="Percentage (%)" fld="13" baseField="10" baseItem="7"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -6835,21 +6822,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44B1C4D-3690-49DE-A0FB-2F661D7F1987}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="29.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.07421875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -6857,210 +6844,156 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B5" s="3">
         <v>63</v>
       </c>
-      <c r="C5" s="3">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B6" s="3">
         <v>71</v>
       </c>
-      <c r="C6" s="3">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="3">
         <v>60</v>
       </c>
-      <c r="C7" s="3">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="3">
         <v>53</v>
       </c>
-      <c r="C8" s="3">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="3">
         <v>54</v>
       </c>
-      <c r="C9" s="3">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="3">
         <v>58</v>
       </c>
-      <c r="C10" s="3">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B11" s="3">
         <v>43</v>
       </c>
-      <c r="C11" s="3">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B12" s="3">
         <v>48</v>
       </c>
-      <c r="C12" s="3">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B13" s="3">
         <v>52</v>
       </c>
-      <c r="C13" s="3">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B14" s="3">
         <v>51</v>
       </c>
-      <c r="C14" s="3">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B15" s="3">
         <v>41</v>
       </c>
-      <c r="C15" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="3">
         <v>50</v>
       </c>
-      <c r="C16" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="3">
         <v>40</v>
       </c>
-      <c r="C17" s="3">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="3">
         <v>14</v>
       </c>
-      <c r="C18" s="3">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B19" s="3">
         <v>39</v>
       </c>
-      <c r="C19" s="3">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B20" s="3">
         <v>18</v>
       </c>
-      <c r="C20" s="3">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B21" s="3">
         <v>42</v>
-      </c>
-      <c r="C21" s="3">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>